<commit_message>
3 op xls generating
</commit_message>
<xml_diff>
--- a/uploads/stockValuation.xlsx
+++ b/uploads/stockValuation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishi\Desktop\Freelance_Projects\priya_fils\backend\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6975F8CE-A3DB-4307-9B60-D533D6BE1F14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D10A63-6126-4ADA-B835-CB651E0B3001}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22255" windowHeight="12646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>QTY IN KGS.</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>BASIC VALUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -358,17 +355,17 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
-        <v>45383</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>45352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -381,149 +378,139 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>173900</v>
+        <v>163575</v>
       </c>
       <c r="B4">
-        <v>99.441184588844166</v>
+        <v>100.77244688980591</v>
       </c>
       <c r="C4">
-        <v>17292822</v>
+        <v>16483853</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2456</v>
+        <v>2645</v>
       </c>
       <c r="B5">
-        <v>239.37988599348535</v>
+        <v>236.51228733459357</v>
       </c>
       <c r="C5">
-        <v>587917</v>
+        <v>625575</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B6">
-        <v>2243.6666666666665</v>
+        <v>2247.3478260869565</v>
       </c>
       <c r="C6">
-        <v>100965</v>
+        <v>103378</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>176401</v>
+        <v>166266</v>
       </c>
       <c r="B7">
-        <v>101.93651963424243</v>
+        <v>103.52571181119411</v>
       </c>
       <c r="C7">
-        <v>17981704</v>
+        <v>17212806</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>43702</v>
+        <v>33018</v>
       </c>
       <c r="B9">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C9">
-        <v>7167128</v>
+        <v>5447970</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>63143</v>
+        <v>65057</v>
       </c>
       <c r="B10">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C10">
-        <v>10355452</v>
+        <v>10734405</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>106845</v>
+        <v>98075</v>
       </c>
       <c r="B11">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C11">
-        <v>17522580</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>3</v>
+        <v>16182375</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>286265</v>
+        <v>294635</v>
       </c>
       <c r="B13">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C13">
-        <v>65268420</v>
+        <v>67471415</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>1576</v>
+        <v>848</v>
       </c>
       <c r="B14">
-        <v>300.32868020304568</v>
+        <v>218.00943396226415</v>
       </c>
       <c r="C14">
-        <v>473318</v>
+        <v>184872</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B15">
+      <c r="A15">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>287841</v>
+        <v>295483</v>
       </c>
       <c r="B16">
-        <v>228.39601724563212</v>
+        <v>228.96845842231195</v>
       </c>
       <c r="C16">
-        <v>65741738</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C19">
-        <v>0</v>
+        <v>67656287</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>571087</v>
+        <v>559824</v>
       </c>
       <c r="B21">
-        <v>177.28651151225645</v>
+        <v>180.50578038812199</v>
       </c>
       <c r="C21">
-        <v>101246022</v>
+        <v>101051468</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>394686</v>
+        <v>393558</v>
       </c>
       <c r="B22">
-        <v>210.96344435830002</v>
+        <v>213.02746228001971</v>
       </c>
       <c r="C22">
-        <v>83264318</v>
+        <v>83838662</v>
       </c>
     </row>
   </sheetData>

</xml_diff>